<commit_message>
add edited traceability matrix
</commit_message>
<xml_diff>
--- a/Monitor and Control/Car-Traceability Matrix.xlsx
+++ b/Monitor and Control/Car-Traceability Matrix.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\QA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -264,28 +272,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <strike/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -295,7 +306,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -304,13 +315,20 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
-    <border/>
+  <borders count="8">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -322,6 +340,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -336,6 +356,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -344,6 +365,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -352,94 +376,95 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -629,545 +654,547 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.86"/>
-    <col customWidth="1" min="2" max="2" width="25.0"/>
-    <col customWidth="1" min="3" max="3" width="24.14"/>
-    <col customWidth="1" min="4" max="26" width="8.71"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" ht="35.25" customHeight="1">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="35.25" customHeight="1">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5"/>
+    </row>
+    <row r="3" spans="1:3" ht="30">
+      <c r="A3" s="11"/>
       <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6" t="s">
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="7"/>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="13"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6" t="s">
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6" t="s">
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="13"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="13"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A21" s="10"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A22" s="12"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="13"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="7"/>
-      <c r="B12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="C23" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A24" s="11"/>
+      <c r="B24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A25" s="11"/>
+      <c r="B25" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="7"/>
-      <c r="B18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="C25" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A26" s="11"/>
+      <c r="B26" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" ht="46.5" customHeight="1">
-      <c r="A27" s="7"/>
-      <c r="B27" s="6" t="s">
+    </row>
+    <row r="27" spans="1:3" ht="46.5" customHeight="1">
+      <c r="A27" s="10"/>
+      <c r="B27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="2" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A28" s="12"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="13"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="6" t="s">
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A30" s="11"/>
+      <c r="B30" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A31" s="11"/>
+      <c r="B31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A32" s="11"/>
+      <c r="B32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A33" s="11"/>
+      <c r="B33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A34" s="11"/>
+      <c r="B34" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A35" s="10"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A36" s="12"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="13"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A37" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="7"/>
-      <c r="B35" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="12"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="8"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="6" t="s">
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A38" s="11"/>
+      <c r="B38" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6" t="s">
+      <c r="C38" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="6" t="s">
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A39" s="11"/>
+      <c r="B39" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A40" s="11"/>
+      <c r="B40" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A41" s="11"/>
+      <c r="B41" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A42" s="11"/>
+      <c r="B42" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A43" s="10"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A44" s="12"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="13"/>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A45" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="7"/>
-      <c r="B43" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="12"/>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="8"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="6" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A46" s="11"/>
+      <c r="B46" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6" t="s">
+      <c r="C46" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6" t="s">
+    </row>
+    <row r="47" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A47" s="11"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="13"/>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="7"/>
-      <c r="B48" s="6" t="s">
+    </row>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A48" s="10"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="12"/>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="8"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="10"/>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="2" t="s">
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A49" s="12"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="13"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A50" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="6" t="s">
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A51" s="11"/>
+      <c r="B51" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="5"/>
-      <c r="B51" s="6" t="s">
+      <c r="C51" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="5"/>
-      <c r="B52" s="6" t="s">
+    </row>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A52" s="11"/>
+      <c r="B52" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="6" t="s">
+    </row>
+    <row r="53" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A53" s="11"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A54" s="11"/>
+      <c r="B54" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A55" s="10"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A56" s="12"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="13"/>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A57" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A58" s="11"/>
+      <c r="B58" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A59" s="11"/>
+      <c r="B59" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="5"/>
-      <c r="B53" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C53" s="13"/>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="5"/>
-      <c r="B54" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="7"/>
-      <c r="B55" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="13"/>
-    </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="8"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="10"/>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="5"/>
-      <c r="B58" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="5"/>
-      <c r="B59" s="6" t="s">
+      <c r="C59" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C59" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="5"/>
-      <c r="B60" s="6" t="s">
+    </row>
+    <row r="60" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A60" s="11"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C60" s="13"/>
-    </row>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="5"/>
-      <c r="B61" s="3" t="s">
+    </row>
+    <row r="61" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A61" s="11"/>
+      <c r="B61" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="7"/>
-      <c r="B62" s="6" t="s">
+    </row>
+    <row r="62" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A62" s="10"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C62" s="13"/>
-    </row>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="64" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -2106,11 +2133,13 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:A18"/>
     <mergeCell ref="A50:A55"/>
     <mergeCell ref="A57:A62"/>
     <mergeCell ref="A28:C28"/>
@@ -2118,17 +2147,13 @@
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A49:C49"/>
     <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="A45:A48"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove cancelled features from traceability matrix
</commit_message>
<xml_diff>
--- a/Monitor and Control/Car-Traceability Matrix.xlsx
+++ b/Monitor and Control/Car-Traceability Matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\QA\QA_project\Car-Bookings\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
   <si>
     <t>CR-ID</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>CR-003</t>
-  </si>
-  <si>
-    <t>SIQ-003</t>
   </si>
   <si>
     <t>CR-004</t>
@@ -88,31 +85,6 @@
     <t xml:space="preserve">SIQ-016 </t>
   </si>
   <si>
-    <t>CR-008</t>
-  </si>
-  <si>
-    <t>CR-009</t>
-  </si>
-  <si>
-    <t>SIQ-006</t>
-  </si>
-  <si>
-    <t>SIQ-010</t>
-  </si>
-  <si>
-    <t>SIQ-013
-SIQ-014</t>
-  </si>
-  <si>
-    <t>CR-010</t>
-  </si>
-  <si>
-    <t>SIQ-005</t>
-  </si>
-  <si>
-    <t>SIQ-013</t>
-  </si>
-  <si>
     <t>Req-Regs-001</t>
   </si>
   <si>
@@ -146,21 +118,6 @@
     <t>Req-User-Log-004</t>
   </si>
   <si>
-    <t>Req-Search-001</t>
-  </si>
-  <si>
-    <t>Req-Search-002</t>
-  </si>
-  <si>
-    <t>Req-Search-003</t>
-  </si>
-  <si>
-    <t>Req-Search-004</t>
-  </si>
-  <si>
-    <t>Req-Search-005</t>
-  </si>
-  <si>
     <t>Req-Res-001</t>
   </si>
   <si>
@@ -182,9 +139,6 @@
     <t>Req-Admin-log-005</t>
   </si>
   <si>
-    <t>Req-Search-006</t>
-  </si>
-  <si>
     <t>Req-Add-Car-001</t>
   </si>
   <si>
@@ -239,48 +193,7 @@
     <t>Req-Del-Car-004</t>
   </si>
   <si>
-    <t>Req-Add-Admin-001</t>
-  </si>
-  <si>
-    <t>Req-Add-Admin-002</t>
-  </si>
-  <si>
-    <t>Req-Add-Admin-003</t>
-  </si>
-  <si>
-    <t>Req-Add-Admin-004</t>
-  </si>
-  <si>
-    <t>Req-Add-Admin-005</t>
-  </si>
-  <si>
-    <t>Req-Add-Admin-006</t>
-  </si>
-  <si>
-    <t>Req-Add-User-001</t>
-  </si>
-  <si>
-    <t>Req-Add-User-002</t>
-  </si>
-  <si>
-    <t>Req-Add-User-003</t>
-  </si>
-  <si>
-    <t>Req-Add-User-004</t>
-  </si>
-  <si>
-    <t>Req-Add-User-005</t>
-  </si>
-  <si>
-    <t>Req-Add-User-006</t>
-  </si>
-  <si>
     <t>Design</t>
-  </si>
-  <si>
-    <t>SQ_User_ColorSearch_03
-SQ_User_BrandSearch_04
-SQ_User_BudgetSearch_05</t>
   </si>
   <si>
     <t>SQ_Admin_AddCar_04
@@ -309,14 +222,6 @@
   <si>
     <t>SQ_Admin_DeleteCar_06
 Car - Delete Car (flow chart)</t>
-  </si>
-  <si>
-    <t>SQ_Admin_AddAdmin_03
-Car - Add Admin (flow chart)</t>
-  </si>
-  <si>
-    <t>SQ_Admin_AddUser_02
-Car - Add User (flow chart)</t>
   </si>
   <si>
     <t xml:space="preserve">Internal Change </t>
@@ -484,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -505,17 +410,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -525,19 +433,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1002"/>
+  <dimension ref="A1:E981"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47:E50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -779,680 +674,482 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="35.25" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="19"/>
+        <v>20</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="17"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="17"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+        <v>22</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="17"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+        <v>23</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="17"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="5"/>
       <c r="C6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+        <v>24</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="17"/>
+      <c r="A7" s="11"/>
       <c r="C7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="18"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="C8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="19"/>
+        <v>27</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="17"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+        <v>28</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="17"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+        <v>29</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="18"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+        <v>30</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A16" s="12"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A18" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="20"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="17"/>
-      <c r="B16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="17"/>
-      <c r="B17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="17"/>
-      <c r="B18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="C18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="17"/>
-      <c r="B19" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A19" s="11"/>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="C19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="18"/>
+        <v>34</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A20" s="11"/>
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A21" s="11"/>
+      <c r="B21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" ht="46.5" customHeight="1">
+      <c r="A22" s="12"/>
+      <c r="B22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A24" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A25" s="11"/>
+      <c r="B25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A26" s="11"/>
+      <c r="B26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A27" s="11"/>
+      <c r="B27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A28" s="11"/>
+      <c r="B28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A29" s="11"/>
+      <c r="B29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A30" s="12"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A31" s="16"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A32" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A33" s="11"/>
+      <c r="B33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A34" s="11"/>
+      <c r="B34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A35" s="11"/>
+      <c r="B35" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A36" s="11"/>
+      <c r="B36" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A37" s="11"/>
+      <c r="B37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A38" s="12"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A39" s="16"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A40" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="20"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A25" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="20"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A26" s="17"/>
-      <c r="B26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A27" s="17"/>
-      <c r="B27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A28" s="17"/>
-      <c r="B28" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-    </row>
-    <row r="29" spans="1:5" ht="46.5" customHeight="1">
-      <c r="A29" s="18"/>
-      <c r="B29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A30" s="13"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A31" s="16" t="s">
+      <c r="D40" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A41" s="11"/>
+      <c r="B41" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" s="19"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A32" s="17"/>
-      <c r="B32" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A42" s="11"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A33" s="17"/>
-      <c r="B33" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="5" t="s">
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A43" s="12"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A34" s="17"/>
-      <c r="B34" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A35" s="17"/>
-      <c r="B35" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A36" s="17"/>
-      <c r="B36" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A37" s="18"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A38" s="13"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A39" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A40" s="17"/>
-      <c r="B40" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A41" s="17"/>
-      <c r="B41" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A42" s="17"/>
-      <c r="B42" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A43" s="17"/>
-      <c r="B43" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A44" s="17"/>
-      <c r="B44" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A45" s="18"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A46" s="13"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A47" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="19"/>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A48" s="17"/>
-      <c r="B48" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-    </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A49" s="17"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A50" s="18"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-    </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A51" s="13"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-    </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A52" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E52" s="19"/>
-    </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A53" s="17"/>
-      <c r="B53" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-    </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A54" s="17"/>
-      <c r="B54" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-    </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A55" s="17"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A56" s="17"/>
-      <c r="B56" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A57" s="18"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A58" s="13"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-    </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A59" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D59" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="E59" s="19"/>
-    </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A60" s="17"/>
-      <c r="B60" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-    </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A61" s="17"/>
-      <c r="B61" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-    </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A62" s="17"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-    </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A63" s="17"/>
-      <c r="B63" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-    </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A64" s="18"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
-    </row>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -2370,68 +2067,35 @@
     <row r="979" ht="15.75" customHeight="1"/>
     <row r="980" ht="15.75" customHeight="1"/>
     <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
-    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E25:E29"/>
-    <mergeCell ref="D59:D64"/>
-    <mergeCell ref="D25:D29"/>
-    <mergeCell ref="D31:D37"/>
-    <mergeCell ref="D39:D45"/>
-    <mergeCell ref="E39:E45"/>
-    <mergeCell ref="E31:E37"/>
-    <mergeCell ref="E47:E50"/>
-    <mergeCell ref="E52:E57"/>
-    <mergeCell ref="E59:E64"/>
-    <mergeCell ref="A59:A64"/>
+  <mergeCells count="27">
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="A40:A43"/>
     <mergeCell ref="D2:D8"/>
     <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D15:D20"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D52:D57"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A31:A37"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A52:A57"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="D24:D30"/>
+    <mergeCell ref="D32:D38"/>
+    <mergeCell ref="E32:E38"/>
+    <mergeCell ref="E24:E30"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E18:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update RTM for Add & update Car TC
</commit_message>
<xml_diff>
--- a/Monitor and Control/Car-Traceability Matrix.xlsx
+++ b/Monitor and Control/Car-Traceability Matrix.xlsx
@@ -5,21 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\QA\QA_project\Car-Bookings\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\QA-Project\Car-Bookings\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7656"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="99">
   <si>
     <t>CR-ID</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>CR-003</t>
+  </si>
+  <si>
+    <t>SIQ-003</t>
   </si>
   <si>
     <t>CR-004</t>
@@ -85,6 +88,31 @@
     <t xml:space="preserve">SIQ-016 </t>
   </si>
   <si>
+    <t>CR-008</t>
+  </si>
+  <si>
+    <t>CR-009</t>
+  </si>
+  <si>
+    <t>SIQ-006</t>
+  </si>
+  <si>
+    <t>SIQ-010</t>
+  </si>
+  <si>
+    <t>SIQ-013
+SIQ-014</t>
+  </si>
+  <si>
+    <t>CR-010</t>
+  </si>
+  <si>
+    <t>SIQ-005</t>
+  </si>
+  <si>
+    <t>SIQ-013</t>
+  </si>
+  <si>
     <t>Req-Regs-001</t>
   </si>
   <si>
@@ -118,6 +146,21 @@
     <t>Req-User-Log-004</t>
   </si>
   <si>
+    <t>Req-Search-001</t>
+  </si>
+  <si>
+    <t>Req-Search-002</t>
+  </si>
+  <si>
+    <t>Req-Search-003</t>
+  </si>
+  <si>
+    <t>Req-Search-004</t>
+  </si>
+  <si>
+    <t>Req-Search-005</t>
+  </si>
+  <si>
     <t>Req-Res-001</t>
   </si>
   <si>
@@ -139,6 +182,9 @@
     <t>Req-Admin-log-005</t>
   </si>
   <si>
+    <t>Req-Search-006</t>
+  </si>
+  <si>
     <t>Req-Add-Car-001</t>
   </si>
   <si>
@@ -193,7 +239,48 @@
     <t>Req-Del-Car-004</t>
   </si>
   <si>
+    <t>Req-Add-Admin-001</t>
+  </si>
+  <si>
+    <t>Req-Add-Admin-002</t>
+  </si>
+  <si>
+    <t>Req-Add-Admin-003</t>
+  </si>
+  <si>
+    <t>Req-Add-Admin-004</t>
+  </si>
+  <si>
+    <t>Req-Add-Admin-005</t>
+  </si>
+  <si>
+    <t>Req-Add-Admin-006</t>
+  </si>
+  <si>
+    <t>Req-Add-User-001</t>
+  </si>
+  <si>
+    <t>Req-Add-User-002</t>
+  </si>
+  <si>
+    <t>Req-Add-User-003</t>
+  </si>
+  <si>
+    <t>Req-Add-User-004</t>
+  </si>
+  <si>
+    <t>Req-Add-User-005</t>
+  </si>
+  <si>
+    <t>Req-Add-User-006</t>
+  </si>
+  <si>
     <t>Design</t>
+  </si>
+  <si>
+    <t>SQ_User_ColorSearch_03
+SQ_User_BrandSearch_04
+SQ_User_BudgetSearch_05</t>
   </si>
   <si>
     <t>SQ_Admin_AddCar_04
@@ -224,10 +311,33 @@
 Car - Delete Car (flow chart)</t>
   </si>
   <si>
+    <t>SQ_Admin_AddAdmin_03
+Car - Add Admin (flow chart)</t>
+  </si>
+  <si>
+    <t>SQ_Admin_AddUser_02
+Car - Add User (flow chart)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Internal Change </t>
   </si>
   <si>
     <t>CR_Des_updateCar_001</t>
+  </si>
+  <si>
+    <t>Test Casess</t>
+  </si>
+  <si>
+    <t>from 
+Car-TC-AddCar-001 
+to 
+Car-TC-AddCar-010</t>
+  </si>
+  <si>
+    <t>from 
+Car-TC-UpdateCar-001
+to
+Car-TC-UpdateCar-009</t>
   </si>
 </sst>
 </file>
@@ -389,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -410,10 +520,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -423,6 +542,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -648,508 +768,777 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E981"/>
+  <dimension ref="A1:F1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40:E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="5" width="26.28515625" customWidth="1"/>
-    <col min="6" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="6" width="26.33203125" customWidth="1"/>
+    <col min="7" max="27" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="35.25" customHeight="1">
+      <c r="A2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:6" ht="28.8">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" ht="14.4">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" ht="14.4">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" ht="14.4">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" ht="14.4">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="D7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" ht="14.4">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.4">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.4">
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" ht="14.4">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" ht="14.4">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" ht="14.4">
+      <c r="A13" s="15"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" ht="14.4">
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" ht="14.4">
+      <c r="A15" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:6" ht="14.4">
+      <c r="A16" s="14"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="1:6" ht="14.4">
+      <c r="A17" s="14"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:6" ht="14.4">
+      <c r="A18" s="14"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="1:6" ht="14.4">
+      <c r="A19" s="14"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="1:6" ht="14.4">
+      <c r="A20" s="15"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="1:6" ht="14.4">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" ht="14.4">
+      <c r="A22" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A23" s="15"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A25" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A26" s="14"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A27" s="14"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A28" s="14"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+    </row>
+    <row r="29" spans="1:6" ht="46.5" customHeight="1">
+      <c r="A29" s="15"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A30" s="20"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A31" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A38" s="20"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A39" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F39" s="13"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="35.25" customHeight="1">
-      <c r="A2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="11"/>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D44" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A46" s="20"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A47" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="11"/>
-      <c r="B4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B47" s="13"/>
+      <c r="C47" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F47" s="13"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A51" s="20"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A52" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="11"/>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B52" s="13"/>
+      <c r="C52" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="11"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4" t="s">
+      <c r="D52" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52" s="13"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="11"/>
-      <c r="C7" s="5" t="s">
+      <c r="D54" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A58" s="20"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A59" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="12"/>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B59" s="13"/>
+      <c r="C59" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="11"/>
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="D59" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F59" s="13"/>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A60" s="14"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A61" s="14"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="11"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="12"/>
-      <c r="B13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A18" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="13"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-    </row>
-    <row r="22" spans="1:5" ht="46.5" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A24" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A30" s="12"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A31" s="16"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A32" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A34" s="11"/>
-      <c r="B34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A35" s="11"/>
-      <c r="B35" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A36" s="11"/>
-      <c r="B36" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A37" s="11"/>
-      <c r="B37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A38" s="12"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A39" s="16"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A40" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E40" s="10"/>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A41" s="11"/>
-      <c r="B41" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A42" s="11"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A43" s="12"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
+      <c r="D63" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A64" s="15"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+    </row>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -2067,35 +2456,78 @@
     <row r="979" ht="15.75" customHeight="1"/>
     <row r="980" ht="15.75" customHeight="1"/>
     <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="A32:A38"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="D24:D30"/>
-    <mergeCell ref="D32:D38"/>
-    <mergeCell ref="E32:E38"/>
-    <mergeCell ref="E24:E30"/>
-    <mergeCell ref="E40:E43"/>
+  <mergeCells count="49">
+    <mergeCell ref="B59:B64"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A31:A37"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A52:A57"/>
+    <mergeCell ref="B31:B37"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B52:B57"/>
+    <mergeCell ref="A59:A64"/>
     <mergeCell ref="E2:E8"/>
     <mergeCell ref="E10:E13"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E18:E22"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="E52:E57"/>
+    <mergeCell ref="E59:E64"/>
+    <mergeCell ref="E25:E29"/>
+    <mergeCell ref="E31:E37"/>
+    <mergeCell ref="E39:E45"/>
+    <mergeCell ref="F39:F45"/>
+    <mergeCell ref="F31:F37"/>
+    <mergeCell ref="F47:F50"/>
+    <mergeCell ref="F52:F57"/>
+    <mergeCell ref="F59:F64"/>
+    <mergeCell ref="F2:F8"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="F15:F20"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F25:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>